<commit_message>
add data download links
</commit_message>
<xml_diff>
--- a/face_detection/symbol_farm/symbol_structures.xlsx
+++ b/face_detection/symbol_farm/symbol_structures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22392" windowHeight="9360" activeTab="1"/>
+    <workbookView windowWidth="22392" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="8" r:id="rId1"/>
@@ -284,10 +284,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -350,22 +350,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -382,17 +366,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -404,8 +389,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -413,7 +413,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,8 +427,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,14 +450,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -464,16 +457,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,7 +501,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,13 +531,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,31 +555,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -573,7 +573,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,55 +651,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,37 +663,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -700,21 +700,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -752,22 +737,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -787,17 +767,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,139 +806,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4011,7 +4011,7 @@
   <sheetPr/>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
@@ -4590,7 +4590,7 @@
   <sheetPr/>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>